<commit_message>
Model 5 Excel updated
</commit_message>
<xml_diff>
--- a/Model.xlsx
+++ b/Model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aditya.Tiwari\Documents\Product Management\Begin AI\TSAI\Repositories\Session 8 assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB64045-EAEF-4D6A-973B-DBCCE1449A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CAD742D-8069-49F2-B265-5D6EBE47F3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="95">
   <si>
     <t>Epoch</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>Reduced layers slightly and added batchnorm. The vanishing gradients problem is resolved, and the model architecuture is as asked for.</t>
+  </si>
+  <si>
+    <t>Conv 6 (d)</t>
   </si>
 </sst>
 </file>
@@ -5196,11 +5199,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5155A9C0-960B-43B5-AA06-FF471900653F}">
-  <dimension ref="C4:S63"/>
+  <dimension ref="C4:S76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S67" sqref="S67"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7868,15 +7871,15 @@
         <v>32</v>
       </c>
       <c r="I52" s="3">
-        <f t="shared" ref="I52:I61" si="50">P51</f>
+        <f t="shared" ref="I52" si="50">P51</f>
         <v>32</v>
       </c>
       <c r="J52" s="3">
-        <f t="shared" ref="J52:J61" si="51">Q51</f>
+        <f t="shared" ref="J52" si="51">Q51</f>
         <v>3</v>
       </c>
       <c r="K52" s="3">
-        <f t="shared" ref="K52:K61" si="52">R51</f>
+        <f t="shared" ref="K52" si="52">R51</f>
         <v>1</v>
       </c>
       <c r="L52" s="3">
@@ -7897,7 +7900,7 @@
         <v>64</v>
       </c>
       <c r="Q52" s="10">
-        <f t="shared" ref="Q52:Q61" si="53">J52+(F52-1)*K52*N52</f>
+        <f t="shared" ref="Q52" si="53">J52+(F52-1)*K52*N52</f>
         <v>5</v>
       </c>
       <c r="R52" s="5">
@@ -8453,11 +8456,11 @@
         <v>1</v>
       </c>
       <c r="O62" s="13">
-        <f t="shared" ref="O53:O62" si="62">FLOOR(((H62+(2*M62)-F62)/L62)+1,1)</f>
+        <f t="shared" ref="O62" si="62">FLOOR(((H62+(2*M62)-F62)/L62)+1,1)</f>
         <v>1</v>
       </c>
       <c r="P62" s="13">
-        <f t="shared" ref="P53:P62" si="63">G62</f>
+        <f t="shared" ref="P62" si="63">G62</f>
         <v>64</v>
       </c>
       <c r="Q62" s="51">
@@ -8495,11 +8498,748 @@
         <v>91</v>
       </c>
     </row>
+    <row r="64" spans="3:19" ht="15" x14ac:dyDescent="0.2">
+      <c r="C64" s="34">
+        <v>6</v>
+      </c>
+      <c r="D64" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F64" s="4">
+        <v>3</v>
+      </c>
+      <c r="G64" s="4">
+        <v>32</v>
+      </c>
+      <c r="H64" s="11">
+        <v>32</v>
+      </c>
+      <c r="I64" s="4">
+        <v>3</v>
+      </c>
+      <c r="J64" s="4">
+        <v>1</v>
+      </c>
+      <c r="K64" s="4">
+        <v>1</v>
+      </c>
+      <c r="L64" s="4">
+        <v>1</v>
+      </c>
+      <c r="M64" s="4">
+        <v>1</v>
+      </c>
+      <c r="N64" s="4">
+        <v>1</v>
+      </c>
+      <c r="O64" s="4">
+        <f t="shared" ref="O64:O76" si="64">FLOOR(((H64+(2*M64)-F64)/L64)+1,1)</f>
+        <v>32</v>
+      </c>
+      <c r="P64" s="4">
+        <f t="shared" ref="P64:P76" si="65">G64</f>
+        <v>32</v>
+      </c>
+      <c r="Q64" s="4">
+        <f>J64+(F64-1)*K64*N64</f>
+        <v>3</v>
+      </c>
+      <c r="R64" s="19">
+        <f t="shared" ref="R64:R75" si="66">K64*L64</f>
+        <v>1</v>
+      </c>
+      <c r="S64" s="46"/>
+    </row>
+    <row r="65" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C65" s="35"/>
+      <c r="D65" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F65" s="3">
+        <v>3</v>
+      </c>
+      <c r="G65" s="3">
+        <v>64</v>
+      </c>
+      <c r="H65" s="3">
+        <f t="shared" ref="H65:H76" si="67">O64</f>
+        <v>32</v>
+      </c>
+      <c r="I65" s="3">
+        <f t="shared" ref="I65:I76" si="68">P64</f>
+        <v>32</v>
+      </c>
+      <c r="J65" s="3">
+        <f t="shared" ref="J65:J76" si="69">Q64</f>
+        <v>3</v>
+      </c>
+      <c r="K65" s="3">
+        <f t="shared" ref="K65:K76" si="70">R64</f>
+        <v>1</v>
+      </c>
+      <c r="L65" s="3">
+        <v>1</v>
+      </c>
+      <c r="M65" s="3">
+        <v>1</v>
+      </c>
+      <c r="N65" s="3">
+        <v>1</v>
+      </c>
+      <c r="O65" s="3">
+        <f t="shared" si="64"/>
+        <v>32</v>
+      </c>
+      <c r="P65" s="3">
+        <f t="shared" si="65"/>
+        <v>64</v>
+      </c>
+      <c r="Q65" s="10">
+        <f t="shared" ref="Q65:Q75" si="71">J65+(F65-1)*K65*N65</f>
+        <v>5</v>
+      </c>
+      <c r="R65" s="5">
+        <f t="shared" si="66"/>
+        <v>1</v>
+      </c>
+      <c r="S65" s="47"/>
+    </row>
+    <row r="66" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C66" s="35"/>
+      <c r="D66" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F66" s="3">
+        <v>2</v>
+      </c>
+      <c r="G66" s="3">
+        <v>64</v>
+      </c>
+      <c r="H66" s="3">
+        <f t="shared" ref="H66:H76" si="72">O65</f>
+        <v>32</v>
+      </c>
+      <c r="I66" s="3">
+        <f t="shared" ref="I66:I76" si="73">P65</f>
+        <v>64</v>
+      </c>
+      <c r="J66" s="3">
+        <f t="shared" ref="J66:J76" si="74">Q65</f>
+        <v>5</v>
+      </c>
+      <c r="K66" s="3">
+        <f t="shared" ref="K66:K76" si="75">R65</f>
+        <v>1</v>
+      </c>
+      <c r="L66" s="3">
+        <v>2</v>
+      </c>
+      <c r="M66" s="3">
+        <v>0</v>
+      </c>
+      <c r="N66" s="3">
+        <v>1</v>
+      </c>
+      <c r="O66" s="3">
+        <f t="shared" ref="O66:O76" si="76">FLOOR(((H66+(2*M66)-F66)/L66)+1,1)</f>
+        <v>16</v>
+      </c>
+      <c r="P66" s="3">
+        <f t="shared" ref="P66:P76" si="77">G66</f>
+        <v>64</v>
+      </c>
+      <c r="Q66" s="10">
+        <f t="shared" ref="Q66:Q76" si="78">J66+(F66-1)*K66*N66</f>
+        <v>6</v>
+      </c>
+      <c r="R66" s="5">
+        <f t="shared" ref="R66:R76" si="79">K66*L66</f>
+        <v>2</v>
+      </c>
+      <c r="S66" s="47"/>
+    </row>
+    <row r="67" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C67" s="35"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F67" s="3">
+        <v>1</v>
+      </c>
+      <c r="G67" s="3">
+        <v>32</v>
+      </c>
+      <c r="H67" s="3">
+        <f t="shared" si="72"/>
+        <v>16</v>
+      </c>
+      <c r="I67" s="3">
+        <f t="shared" si="73"/>
+        <v>64</v>
+      </c>
+      <c r="J67" s="3">
+        <f t="shared" si="74"/>
+        <v>6</v>
+      </c>
+      <c r="K67" s="3">
+        <f t="shared" si="75"/>
+        <v>2</v>
+      </c>
+      <c r="L67" s="3">
+        <v>1</v>
+      </c>
+      <c r="M67" s="3">
+        <v>0</v>
+      </c>
+      <c r="N67" s="3">
+        <v>1</v>
+      </c>
+      <c r="O67" s="3">
+        <f t="shared" si="76"/>
+        <v>16</v>
+      </c>
+      <c r="P67" s="3">
+        <f t="shared" si="77"/>
+        <v>32</v>
+      </c>
+      <c r="Q67" s="10">
+        <f t="shared" si="78"/>
+        <v>6</v>
+      </c>
+      <c r="R67" s="5">
+        <f t="shared" si="79"/>
+        <v>2</v>
+      </c>
+      <c r="S67" s="47"/>
+    </row>
+    <row r="68" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C68" s="35"/>
+      <c r="D68" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F68" s="3">
+        <v>3</v>
+      </c>
+      <c r="G68" s="3">
+        <v>64</v>
+      </c>
+      <c r="H68" s="3">
+        <f t="shared" si="72"/>
+        <v>16</v>
+      </c>
+      <c r="I68" s="3">
+        <f t="shared" si="73"/>
+        <v>32</v>
+      </c>
+      <c r="J68" s="3">
+        <f t="shared" si="74"/>
+        <v>6</v>
+      </c>
+      <c r="K68" s="3">
+        <f t="shared" si="75"/>
+        <v>2</v>
+      </c>
+      <c r="L68" s="3">
+        <v>1</v>
+      </c>
+      <c r="M68" s="3">
+        <v>1</v>
+      </c>
+      <c r="N68" s="3">
+        <v>1</v>
+      </c>
+      <c r="O68" s="3">
+        <f t="shared" si="76"/>
+        <v>16</v>
+      </c>
+      <c r="P68" s="3">
+        <f t="shared" si="77"/>
+        <v>64</v>
+      </c>
+      <c r="Q68" s="10">
+        <f t="shared" si="78"/>
+        <v>10</v>
+      </c>
+      <c r="R68" s="5">
+        <f t="shared" si="79"/>
+        <v>2</v>
+      </c>
+      <c r="S68" s="47"/>
+    </row>
+    <row r="69" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C69" s="35"/>
+      <c r="D69" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F69" s="3">
+        <v>2</v>
+      </c>
+      <c r="G69" s="3">
+        <v>64</v>
+      </c>
+      <c r="H69" s="3">
+        <f t="shared" si="72"/>
+        <v>16</v>
+      </c>
+      <c r="I69" s="3">
+        <f t="shared" si="73"/>
+        <v>64</v>
+      </c>
+      <c r="J69" s="3">
+        <f t="shared" si="74"/>
+        <v>10</v>
+      </c>
+      <c r="K69" s="3">
+        <f t="shared" si="75"/>
+        <v>2</v>
+      </c>
+      <c r="L69" s="3">
+        <v>2</v>
+      </c>
+      <c r="M69" s="3">
+        <v>0</v>
+      </c>
+      <c r="N69" s="3">
+        <v>1</v>
+      </c>
+      <c r="O69" s="3">
+        <f t="shared" si="76"/>
+        <v>8</v>
+      </c>
+      <c r="P69" s="3">
+        <f t="shared" si="77"/>
+        <v>64</v>
+      </c>
+      <c r="Q69" s="10">
+        <f t="shared" si="78"/>
+        <v>12</v>
+      </c>
+      <c r="R69" s="5">
+        <f t="shared" si="79"/>
+        <v>4</v>
+      </c>
+      <c r="S69" s="47"/>
+    </row>
+    <row r="70" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C70" s="35"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F70" s="3">
+        <v>1</v>
+      </c>
+      <c r="G70" s="3">
+        <v>32</v>
+      </c>
+      <c r="H70" s="3">
+        <f t="shared" si="72"/>
+        <v>8</v>
+      </c>
+      <c r="I70" s="3">
+        <f t="shared" si="73"/>
+        <v>64</v>
+      </c>
+      <c r="J70" s="3">
+        <f t="shared" si="74"/>
+        <v>12</v>
+      </c>
+      <c r="K70" s="3">
+        <f t="shared" si="75"/>
+        <v>4</v>
+      </c>
+      <c r="L70" s="3">
+        <v>1</v>
+      </c>
+      <c r="M70" s="3">
+        <v>0</v>
+      </c>
+      <c r="N70" s="3">
+        <v>1</v>
+      </c>
+      <c r="O70" s="3">
+        <f t="shared" si="76"/>
+        <v>8</v>
+      </c>
+      <c r="P70" s="3">
+        <f t="shared" si="77"/>
+        <v>32</v>
+      </c>
+      <c r="Q70" s="10">
+        <f t="shared" si="78"/>
+        <v>12</v>
+      </c>
+      <c r="R70" s="5">
+        <f t="shared" si="79"/>
+        <v>4</v>
+      </c>
+      <c r="S70" s="47"/>
+    </row>
+    <row r="71" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C71" s="35"/>
+      <c r="D71" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F71" s="3">
+        <v>3</v>
+      </c>
+      <c r="G71" s="3">
+        <v>64</v>
+      </c>
+      <c r="H71" s="3">
+        <f t="shared" si="72"/>
+        <v>8</v>
+      </c>
+      <c r="I71" s="3">
+        <f t="shared" si="73"/>
+        <v>32</v>
+      </c>
+      <c r="J71" s="3">
+        <f t="shared" si="74"/>
+        <v>12</v>
+      </c>
+      <c r="K71" s="3">
+        <f t="shared" si="75"/>
+        <v>4</v>
+      </c>
+      <c r="L71" s="3">
+        <v>1</v>
+      </c>
+      <c r="M71" s="3">
+        <v>1</v>
+      </c>
+      <c r="N71" s="3">
+        <v>2</v>
+      </c>
+      <c r="O71" s="3">
+        <f t="shared" si="76"/>
+        <v>8</v>
+      </c>
+      <c r="P71" s="3">
+        <f t="shared" si="77"/>
+        <v>64</v>
+      </c>
+      <c r="Q71" s="10">
+        <f t="shared" si="78"/>
+        <v>28</v>
+      </c>
+      <c r="R71" s="5">
+        <f t="shared" si="79"/>
+        <v>4</v>
+      </c>
+      <c r="S71" s="47"/>
+    </row>
+    <row r="72" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C72" s="35"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F72" s="3">
+        <v>3</v>
+      </c>
+      <c r="G72" s="3">
+        <v>64</v>
+      </c>
+      <c r="H72" s="3">
+        <f t="shared" si="72"/>
+        <v>8</v>
+      </c>
+      <c r="I72" s="3">
+        <f t="shared" si="73"/>
+        <v>64</v>
+      </c>
+      <c r="J72" s="3">
+        <f t="shared" si="74"/>
+        <v>28</v>
+      </c>
+      <c r="K72" s="3">
+        <f t="shared" si="75"/>
+        <v>4</v>
+      </c>
+      <c r="L72" s="13">
+        <v>1</v>
+      </c>
+      <c r="M72" s="13">
+        <v>1</v>
+      </c>
+      <c r="N72" s="13">
+        <v>1</v>
+      </c>
+      <c r="O72" s="3">
+        <f t="shared" si="76"/>
+        <v>8</v>
+      </c>
+      <c r="P72" s="3">
+        <f t="shared" si="77"/>
+        <v>64</v>
+      </c>
+      <c r="Q72" s="10">
+        <f t="shared" si="78"/>
+        <v>36</v>
+      </c>
+      <c r="R72" s="5">
+        <f t="shared" si="79"/>
+        <v>4</v>
+      </c>
+      <c r="S72" s="47"/>
+    </row>
+    <row r="73" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C73" s="35"/>
+      <c r="D73" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="F73" s="3">
+        <v>2</v>
+      </c>
+      <c r="G73" s="3">
+        <v>64</v>
+      </c>
+      <c r="H73" s="3">
+        <f t="shared" si="72"/>
+        <v>8</v>
+      </c>
+      <c r="I73" s="3">
+        <f t="shared" si="73"/>
+        <v>64</v>
+      </c>
+      <c r="J73" s="3">
+        <f t="shared" si="74"/>
+        <v>36</v>
+      </c>
+      <c r="K73" s="3">
+        <f t="shared" si="75"/>
+        <v>4</v>
+      </c>
+      <c r="L73" s="13">
+        <v>2</v>
+      </c>
+      <c r="M73" s="13">
+        <v>0</v>
+      </c>
+      <c r="N73" s="13">
+        <v>1</v>
+      </c>
+      <c r="O73" s="3">
+        <f t="shared" si="76"/>
+        <v>4</v>
+      </c>
+      <c r="P73" s="3">
+        <f t="shared" si="77"/>
+        <v>64</v>
+      </c>
+      <c r="Q73" s="10">
+        <f t="shared" si="78"/>
+        <v>40</v>
+      </c>
+      <c r="R73" s="5">
+        <f t="shared" si="79"/>
+        <v>8</v>
+      </c>
+      <c r="S73" s="47"/>
+    </row>
+    <row r="74" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C74" s="35"/>
+      <c r="D74" s="39"/>
+      <c r="E74" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F74" s="3">
+        <v>1</v>
+      </c>
+      <c r="G74" s="3">
+        <v>32</v>
+      </c>
+      <c r="H74" s="3">
+        <f t="shared" si="72"/>
+        <v>4</v>
+      </c>
+      <c r="I74" s="3">
+        <f t="shared" si="73"/>
+        <v>64</v>
+      </c>
+      <c r="J74" s="3">
+        <f t="shared" si="74"/>
+        <v>40</v>
+      </c>
+      <c r="K74" s="3">
+        <f t="shared" si="75"/>
+        <v>8</v>
+      </c>
+      <c r="L74" s="13">
+        <v>1</v>
+      </c>
+      <c r="M74" s="13">
+        <v>0</v>
+      </c>
+      <c r="N74" s="13">
+        <v>1</v>
+      </c>
+      <c r="O74" s="3">
+        <f t="shared" si="76"/>
+        <v>4</v>
+      </c>
+      <c r="P74" s="3">
+        <f t="shared" si="77"/>
+        <v>32</v>
+      </c>
+      <c r="Q74" s="10">
+        <f t="shared" si="78"/>
+        <v>40</v>
+      </c>
+      <c r="R74" s="5">
+        <f t="shared" si="79"/>
+        <v>8</v>
+      </c>
+      <c r="S74" s="47"/>
+    </row>
+    <row r="75" spans="3:19" x14ac:dyDescent="0.2">
+      <c r="C75" s="35"/>
+      <c r="D75" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="E75" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F75" s="13">
+        <v>3</v>
+      </c>
+      <c r="G75" s="13">
+        <v>64</v>
+      </c>
+      <c r="H75" s="3">
+        <f t="shared" si="72"/>
+        <v>4</v>
+      </c>
+      <c r="I75" s="3">
+        <f t="shared" si="73"/>
+        <v>32</v>
+      </c>
+      <c r="J75" s="3">
+        <f t="shared" si="74"/>
+        <v>40</v>
+      </c>
+      <c r="K75" s="3">
+        <f t="shared" si="75"/>
+        <v>8</v>
+      </c>
+      <c r="L75" s="13">
+        <v>1</v>
+      </c>
+      <c r="M75" s="13">
+        <v>1</v>
+      </c>
+      <c r="N75" s="13">
+        <v>1</v>
+      </c>
+      <c r="O75" s="3">
+        <f t="shared" si="76"/>
+        <v>4</v>
+      </c>
+      <c r="P75" s="3">
+        <f t="shared" si="77"/>
+        <v>64</v>
+      </c>
+      <c r="Q75" s="10">
+        <f t="shared" si="78"/>
+        <v>56</v>
+      </c>
+      <c r="R75" s="5">
+        <f t="shared" si="79"/>
+        <v>8</v>
+      </c>
+      <c r="S75" s="47"/>
+    </row>
+    <row r="76" spans="3:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="36"/>
+      <c r="D76" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F76" s="6">
+        <v>4</v>
+      </c>
+      <c r="G76" s="6">
+        <v>64</v>
+      </c>
+      <c r="H76" s="3">
+        <f t="shared" si="72"/>
+        <v>4</v>
+      </c>
+      <c r="I76" s="3">
+        <f t="shared" si="73"/>
+        <v>64</v>
+      </c>
+      <c r="J76" s="3">
+        <f t="shared" si="74"/>
+        <v>56</v>
+      </c>
+      <c r="K76" s="3">
+        <f t="shared" si="75"/>
+        <v>8</v>
+      </c>
+      <c r="L76" s="6">
+        <v>1</v>
+      </c>
+      <c r="M76" s="6">
+        <v>0</v>
+      </c>
+      <c r="N76" s="6">
+        <v>1</v>
+      </c>
+      <c r="O76" s="3">
+        <f t="shared" si="76"/>
+        <v>1</v>
+      </c>
+      <c r="P76" s="3">
+        <f t="shared" si="77"/>
+        <v>64</v>
+      </c>
+      <c r="Q76" s="10">
+        <f>Q75</f>
+        <v>56</v>
+      </c>
+      <c r="R76" s="5">
+        <f t="shared" si="79"/>
+        <v>8</v>
+      </c>
+      <c r="S76" s="48"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="34">
     <mergeCell ref="D63:R63"/>
     <mergeCell ref="D28:D29"/>
     <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C64:C76"/>
+    <mergeCell ref="S64:S76"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="D71:D72"/>
     <mergeCell ref="S6:S25"/>
     <mergeCell ref="S26:S34"/>
     <mergeCell ref="S35:S50"/>
@@ -8536,7 +9276,7 @@
   <dimension ref="D1:Q402"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
@@ -14642,7 +15382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7711C3A-5153-46B1-ADD9-E0A1899966C0}">
   <dimension ref="G2:AA22"/>
   <sheetViews>
-    <sheetView topLeftCell="F24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="F6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Z33" sqref="Z33"/>
     </sheetView>
   </sheetViews>

</xml_diff>